<commit_message>
reporting manager excel import
</commit_message>
<xml_diff>
--- a/public/uploads/files/employees.xlsx
+++ b/public/uploads/files/employees.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aayus\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E77A244-1427-4DCE-A8AB-5985AADFC8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -58,46 +67,53 @@
     <t>Ashmita Srivastava</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>ashmita.shrivastava@niletechnologies.com</t>
-    </r>
-  </si>
-  <si>
     <t>Android Developer</t>
   </si>
   <si>
     <t>Aayushi Sinha</t>
   </si>
   <si>
-    <t>aayushi.sinha319@gmail.com</t>
-  </si>
-  <si>
     <t>Software Developer</t>
+  </si>
+  <si>
+    <t>ashmita.shrivastava@niletechnologies.com</t>
+  </si>
+  <si>
+    <t>aayushi.sinha@niletechnologies.com</t>
+  </si>
+  <si>
+    <t>Reporting Manager</t>
+  </si>
+  <si>
+    <t>Preeti Malhotra</t>
+  </si>
+  <si>
+    <t>Payal Chhikara</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,39 +121,46 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -327,125 +350,143 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1329</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>8.240147455E9</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1">
+        <v>8240147455</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
-        <v>1329.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1255</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>1.23456789E9</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
-        <v>1255.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1312</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1">
-        <v>8.054457101E9</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1">
+        <v>8054457101</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1">
-        <v>1312.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1378</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1">
-        <v>7.668373069E9</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1">
+        <v>7668373069</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1357</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1">
-        <v>1378.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="1">
+        <v>9155857561</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="1">
-        <v>9.155857561E9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1357.0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C5"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{B86DC150-356A-4E58-93E6-6DF57F2B7D80}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>